<commit_message>
S_AGILE_02: Conduct Sprint Planning
</commit_message>
<xml_diff>
--- a/agile_crash_course/backlog_sample_creation.xlsx
+++ b/agile_crash_course/backlog_sample_creation.xlsx
@@ -182,7 +182,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -223,6 +223,7 @@
       <color rgb="FF000000"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -230,12 +231,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF999999"/>
-      <name val="Cambria"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -327,11 +322,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -571,10 +566,10 @@
   </sheetPr>
   <dimension ref="A1:AC1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>